<commit_message>
done auto write to ggsheet and cal total hour of each staff
</commit_message>
<xml_diff>
--- a/server/database/data_per_month/10-2025.xlsx
+++ b/server/database/data_per_month/10-2025.xlsx
@@ -621,7 +621,11 @@
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>|10:46-13:00(No thing)|13:41-13:45()|</t>
+          <t xml:space="preserve">14:54-14:55(No thing)
+14:55-14:59(No thing)
+15:00-15:01(No thing)
+15:02-15:02(No thing)
+</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr"/>
@@ -629,7 +633,11 @@
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -779,11 +787,7 @@
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>|13:30-13:32(No thing)|13:33-13:33(No thing)|13:35-13:38(No thing)|</t>
-        </is>
-      </c>
+      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="inlineStr"/>

</xml_diff>